<commit_message>
Base layer rectangles on actual global coord position
</commit_message>
<xml_diff>
--- a/TRDDimensions.xlsx
+++ b/TRDDimensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\alice\jsroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85E2983-EA54-47BA-8DC0-182A688C7DA0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3939EC3D-CE7C-42E9-B769-158787688E8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
   <si>
     <t>Layer</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>area</t>
+  </si>
+  <si>
+    <t>minR</t>
+  </si>
+  <si>
+    <t>maxR</t>
   </si>
 </sst>
 </file>
@@ -1972,15 +1978,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="O4" sqref="O4:O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2018,7 +2024,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2056,7 +2062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2096,8 +2102,14 @@
       <c r="M3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2137,8 +2149,14 @@
       <c r="M4">
         <v>2925</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>2945</v>
+      </c>
+      <c r="O4">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2178,8 +2196,14 @@
       <c r="M5">
         <v>2925</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5">
+        <v>2945</v>
+      </c>
+      <c r="O5">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2219,8 +2243,14 @@
       <c r="M6">
         <v>2925</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6">
+        <v>2945</v>
+      </c>
+      <c r="O6">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2260,8 +2290,14 @@
       <c r="M7">
         <v>2925</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7">
+        <v>2945</v>
+      </c>
+      <c r="O7">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2301,8 +2337,14 @@
       <c r="M8">
         <v>2925</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8">
+        <v>2945</v>
+      </c>
+      <c r="O8">
+        <v>3065</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2342,8 +2384,14 @@
       <c r="M9">
         <v>3065</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <v>3071</v>
+      </c>
+      <c r="O9">
+        <v>3191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2383,8 +2431,14 @@
       <c r="M10">
         <v>3065</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N10">
+        <v>3071</v>
+      </c>
+      <c r="O10">
+        <v>3191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2424,8 +2478,14 @@
       <c r="M11">
         <v>3065</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N11">
+        <v>3071</v>
+      </c>
+      <c r="O11">
+        <v>3191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2465,8 +2525,14 @@
       <c r="M12">
         <v>3065</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12">
+        <v>3071</v>
+      </c>
+      <c r="O12">
+        <v>3191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2506,8 +2572,14 @@
       <c r="M13">
         <v>3065</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N13">
+        <v>3071</v>
+      </c>
+      <c r="O13">
+        <v>3191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2547,8 +2619,14 @@
       <c r="M14">
         <v>3203</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N14">
+        <v>3197</v>
+      </c>
+      <c r="O14">
+        <v>3317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2588,8 +2666,14 @@
       <c r="M15">
         <v>3203</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N15">
+        <v>3197</v>
+      </c>
+      <c r="O15">
+        <v>3317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2629,8 +2713,14 @@
       <c r="M16">
         <v>3203</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N16">
+        <v>3197</v>
+      </c>
+      <c r="O16">
+        <v>3317</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2670,8 +2760,14 @@
       <c r="M17">
         <v>3203</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N17">
+        <v>3197</v>
+      </c>
+      <c r="O17">
+        <v>3317</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2711,8 +2807,14 @@
       <c r="M18">
         <v>3203</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N18">
+        <v>3197</v>
+      </c>
+      <c r="O18">
+        <v>3317</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2752,8 +2854,14 @@
       <c r="M19">
         <v>3340</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N19">
+        <v>3323</v>
+      </c>
+      <c r="O19">
+        <v>3443</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2793,8 +2901,14 @@
       <c r="M20">
         <v>3340</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N20">
+        <v>3323</v>
+      </c>
+      <c r="O20">
+        <v>3443</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2834,8 +2948,14 @@
       <c r="M21">
         <v>3340</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N21">
+        <v>3323</v>
+      </c>
+      <c r="O21">
+        <v>3443</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2875,8 +2995,14 @@
       <c r="M22">
         <v>3340</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N22">
+        <v>3323</v>
+      </c>
+      <c r="O22">
+        <v>3443</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2916,8 +3042,14 @@
       <c r="M23">
         <v>3340</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N23">
+        <v>3323</v>
+      </c>
+      <c r="O23">
+        <v>3443</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
@@ -2957,8 +3089,14 @@
       <c r="M24">
         <v>3481</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N24">
+        <v>3449</v>
+      </c>
+      <c r="O24">
+        <v>3569</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
@@ -2998,8 +3136,14 @@
       <c r="M25">
         <v>3481</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N25">
+        <v>3449</v>
+      </c>
+      <c r="O25">
+        <v>3569</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3039,8 +3183,14 @@
       <c r="M26">
         <v>3481</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N26">
+        <v>3449</v>
+      </c>
+      <c r="O26">
+        <v>3569</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4</v>
       </c>
@@ -3080,8 +3230,14 @@
       <c r="M27">
         <v>3481</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N27">
+        <v>3449</v>
+      </c>
+      <c r="O27">
+        <v>3569</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
@@ -3121,8 +3277,14 @@
       <c r="M28">
         <v>3481</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N28">
+        <v>3449</v>
+      </c>
+      <c r="O28">
+        <v>3569</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
@@ -3162,8 +3324,14 @@
       <c r="M29">
         <v>3618</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N29">
+        <v>3575</v>
+      </c>
+      <c r="O29">
+        <v>3695</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5</v>
       </c>
@@ -3203,8 +3371,14 @@
       <c r="M30">
         <v>3618</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N30">
+        <v>3575</v>
+      </c>
+      <c r="O30">
+        <v>3695</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>5</v>
       </c>
@@ -3244,8 +3418,14 @@
       <c r="M31">
         <v>3618</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N31">
+        <v>3575</v>
+      </c>
+      <c r="O31">
+        <v>3695</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>5</v>
       </c>
@@ -3285,8 +3465,14 @@
       <c r="M32">
         <v>3618</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N32">
+        <v>3575</v>
+      </c>
+      <c r="O32">
+        <v>3695</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>5</v>
       </c>
@@ -3325,6 +3511,12 @@
       </c>
       <c r="M33">
         <v>3618</v>
+      </c>
+      <c r="N33">
+        <v>3575</v>
+      </c>
+      <c r="O33">
+        <v>3695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rescale detector radius measurements to cm
</commit_message>
<xml_diff>
--- a/TRDDimensions.xlsx
+++ b/TRDDimensions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\alice\jsroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3939EC3D-CE7C-42E9-B769-158787688E8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987DBCD6-9BEF-43F5-8D04-88EEB41DDA03}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1980,9 +1980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:O33"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -2150,10 +2148,10 @@
         <v>2925</v>
       </c>
       <c r="N4">
-        <v>2945</v>
+        <v>294.5</v>
       </c>
       <c r="O4">
-        <v>3065</v>
+        <v>306.5</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -2197,10 +2195,10 @@
         <v>2925</v>
       </c>
       <c r="N5">
-        <v>2945</v>
+        <v>294.5</v>
       </c>
       <c r="O5">
-        <v>3065</v>
+        <v>306.5</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -2244,10 +2242,10 @@
         <v>2925</v>
       </c>
       <c r="N6">
-        <v>2945</v>
+        <v>294.5</v>
       </c>
       <c r="O6">
-        <v>3065</v>
+        <v>306.5</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -2291,10 +2289,10 @@
         <v>2925</v>
       </c>
       <c r="N7">
-        <v>2945</v>
+        <v>294.5</v>
       </c>
       <c r="O7">
-        <v>3065</v>
+        <v>306.5</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2338,10 +2336,10 @@
         <v>2925</v>
       </c>
       <c r="N8">
-        <v>2945</v>
+        <v>294.5</v>
       </c>
       <c r="O8">
-        <v>3065</v>
+        <v>306.5</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2385,10 +2383,10 @@
         <v>3065</v>
       </c>
       <c r="N9">
-        <v>3071</v>
+        <v>307.10000000000002</v>
       </c>
       <c r="O9">
-        <v>3191</v>
+        <v>319.10000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -2432,10 +2430,10 @@
         <v>3065</v>
       </c>
       <c r="N10">
-        <v>3071</v>
+        <v>307.10000000000002</v>
       </c>
       <c r="O10">
-        <v>3191</v>
+        <v>319.10000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2479,10 +2477,10 @@
         <v>3065</v>
       </c>
       <c r="N11">
-        <v>3071</v>
+        <v>307.10000000000002</v>
       </c>
       <c r="O11">
-        <v>3191</v>
+        <v>319.10000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2526,10 +2524,10 @@
         <v>3065</v>
       </c>
       <c r="N12">
-        <v>3071</v>
+        <v>307.10000000000002</v>
       </c>
       <c r="O12">
-        <v>3191</v>
+        <v>319.10000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2573,10 +2571,10 @@
         <v>3065</v>
       </c>
       <c r="N13">
-        <v>3071</v>
+        <v>307.10000000000002</v>
       </c>
       <c r="O13">
-        <v>3191</v>
+        <v>319.10000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -2620,10 +2618,10 @@
         <v>3203</v>
       </c>
       <c r="N14">
-        <v>3197</v>
+        <v>319.7</v>
       </c>
       <c r="O14">
-        <v>3317</v>
+        <v>331.7</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -2667,10 +2665,10 @@
         <v>3203</v>
       </c>
       <c r="N15">
-        <v>3197</v>
+        <v>319.7</v>
       </c>
       <c r="O15">
-        <v>3317</v>
+        <v>331.7</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -2714,10 +2712,10 @@
         <v>3203</v>
       </c>
       <c r="N16">
-        <v>3197</v>
+        <v>319.7</v>
       </c>
       <c r="O16">
-        <v>3317</v>
+        <v>331.7</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -2761,10 +2759,10 @@
         <v>3203</v>
       </c>
       <c r="N17">
-        <v>3197</v>
+        <v>319.7</v>
       </c>
       <c r="O17">
-        <v>3317</v>
+        <v>331.7</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -2808,10 +2806,10 @@
         <v>3203</v>
       </c>
       <c r="N18">
-        <v>3197</v>
+        <v>319.7</v>
       </c>
       <c r="O18">
-        <v>3317</v>
+        <v>331.7</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -2855,10 +2853,10 @@
         <v>3340</v>
       </c>
       <c r="N19">
-        <v>3323</v>
+        <v>332.3</v>
       </c>
       <c r="O19">
-        <v>3443</v>
+        <v>344.3</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -2902,10 +2900,10 @@
         <v>3340</v>
       </c>
       <c r="N20">
-        <v>3323</v>
+        <v>332.3</v>
       </c>
       <c r="O20">
-        <v>3443</v>
+        <v>344.3</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -2949,10 +2947,10 @@
         <v>3340</v>
       </c>
       <c r="N21">
-        <v>3323</v>
+        <v>332.3</v>
       </c>
       <c r="O21">
-        <v>3443</v>
+        <v>344.3</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -2996,10 +2994,10 @@
         <v>3340</v>
       </c>
       <c r="N22">
-        <v>3323</v>
+        <v>332.3</v>
       </c>
       <c r="O22">
-        <v>3443</v>
+        <v>344.3</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -3043,10 +3041,10 @@
         <v>3340</v>
       </c>
       <c r="N23">
-        <v>3323</v>
+        <v>332.3</v>
       </c>
       <c r="O23">
-        <v>3443</v>
+        <v>344.3</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -3090,10 +3088,10 @@
         <v>3481</v>
       </c>
       <c r="N24">
-        <v>3449</v>
+        <v>344.9</v>
       </c>
       <c r="O24">
-        <v>3569</v>
+        <v>356.9</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -3137,10 +3135,10 @@
         <v>3481</v>
       </c>
       <c r="N25">
-        <v>3449</v>
+        <v>344.9</v>
       </c>
       <c r="O25">
-        <v>3569</v>
+        <v>356.9</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -3184,10 +3182,10 @@
         <v>3481</v>
       </c>
       <c r="N26">
-        <v>3449</v>
+        <v>344.9</v>
       </c>
       <c r="O26">
-        <v>3569</v>
+        <v>356.9</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -3231,10 +3229,10 @@
         <v>3481</v>
       </c>
       <c r="N27">
-        <v>3449</v>
+        <v>344.9</v>
       </c>
       <c r="O27">
-        <v>3569</v>
+        <v>356.9</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -3278,10 +3276,10 @@
         <v>3481</v>
       </c>
       <c r="N28">
-        <v>3449</v>
+        <v>344.9</v>
       </c>
       <c r="O28">
-        <v>3569</v>
+        <v>356.9</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -3325,10 +3323,10 @@
         <v>3618</v>
       </c>
       <c r="N29">
-        <v>3575</v>
+        <v>357.5</v>
       </c>
       <c r="O29">
-        <v>3695</v>
+        <v>369.5</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -3372,10 +3370,10 @@
         <v>3618</v>
       </c>
       <c r="N30">
-        <v>3575</v>
+        <v>357.5</v>
       </c>
       <c r="O30">
-        <v>3695</v>
+        <v>369.5</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -3419,10 +3417,10 @@
         <v>3618</v>
       </c>
       <c r="N31">
-        <v>3575</v>
+        <v>357.5</v>
       </c>
       <c r="O31">
-        <v>3695</v>
+        <v>369.5</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -3466,10 +3464,10 @@
         <v>3618</v>
       </c>
       <c r="N32">
-        <v>3575</v>
+        <v>357.5</v>
       </c>
       <c r="O32">
-        <v>3695</v>
+        <v>369.5</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -3513,10 +3511,10 @@
         <v>3618</v>
       </c>
       <c r="N33">
-        <v>3575</v>
+        <v>357.5</v>
       </c>
       <c r="O33">
-        <v>3695</v>
+        <v>369.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add z-dimensions, rename module to stack
</commit_message>
<xml_diff>
--- a/TRDDimensions.xlsx
+++ b/TRDDimensions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\alice\jsroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987DBCD6-9BEF-43F5-8D04-88EEB41DDA03}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D43F83E-572B-4758-882F-502CBA14CC98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-4680" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
   <si>
     <t>Layer</t>
   </si>
@@ -129,14 +129,23 @@
   <si>
     <t>maxR</t>
   </si>
+  <si>
+    <t>minZ</t>
+  </si>
+  <si>
+    <t>maxZ</t>
+  </si>
+  <si>
+    <t>zrange_round</t>
+  </si>
+  <si>
+    <t>stack</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,11 +175,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,26 +491,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A1:M33"/>
+      <selection activeCell="P1" sqref="P1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
-    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,10 +516,10 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -542,7 +537,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -580,7 +575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -591,7 +586,7 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -620,1355 +615,1838 @@
       <c r="M3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>93.6</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>120.5</v>
       </c>
       <c r="E4">
         <v>16</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
+        <v>7.53</v>
+      </c>
+      <c r="G4">
         <v>0.65</v>
       </c>
-      <c r="G4" s="1">
-        <v>7.53</v>
-      </c>
-      <c r="H4" s="3">
-        <v>144</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="H4">
+        <v>144</v>
+      </c>
+      <c r="I4">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J4" s="1">
-        <f t="shared" ref="J4:J33" si="0">-C4/2</f>
+      <c r="J4">
         <v>-46.8</v>
       </c>
-      <c r="K4" s="1">
-        <f t="shared" ref="K4:K33" si="1">C4/2</f>
+      <c r="K4">
         <v>46.8</v>
       </c>
       <c r="L4">
-        <f>ROUNDDOWN(J4/0.016, 0)</f>
         <v>-2925</v>
       </c>
       <c r="M4">
-        <f>ROUNDDOWN(K4/0.016, 0)</f>
         <v>2925</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4">
+        <v>294.5</v>
+      </c>
+      <c r="O4">
+        <v>306.5</v>
+      </c>
+      <c r="P4">
+        <f>Q4-E4*F4</f>
+        <v>-294.42</v>
+      </c>
+      <c r="Q4">
+        <f>P5</f>
+        <v>-173.94</v>
+      </c>
+      <c r="R4">
+        <f>E4*F4</f>
+        <v>120.48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>93.6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>120.5</v>
       </c>
       <c r="E5">
         <v>16</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
+        <v>7.53</v>
+      </c>
+      <c r="G5">
         <v>0.65</v>
       </c>
-      <c r="G5" s="1">
-        <v>7.53</v>
-      </c>
-      <c r="H5" s="3">
-        <v>144</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="H5">
+        <v>144</v>
+      </c>
+      <c r="I5">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J5" s="1">
-        <f t="shared" si="0"/>
+      <c r="J5">
         <v>-46.8</v>
       </c>
-      <c r="K5" s="1">
-        <f t="shared" si="1"/>
+      <c r="K5">
         <v>46.8</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L33" si="2">ROUNDDOWN(J5/0.016, 0)</f>
         <v>-2925</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M33" si="3">ROUNDDOWN(K5/0.016, 0)</f>
         <v>2925</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5">
+        <v>294.5</v>
+      </c>
+      <c r="O5">
+        <v>306.5</v>
+      </c>
+      <c r="P5">
+        <f>Q5-E5*F5</f>
+        <v>-173.94</v>
+      </c>
+      <c r="Q5">
+        <f>P6</f>
+        <v>-53.46</v>
+      </c>
+      <c r="R5">
+        <f>E5*F5</f>
+        <v>120.48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>93.6</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>107</v>
       </c>
       <c r="E6">
         <v>12</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
+        <v>8.91</v>
+      </c>
+      <c r="G6">
         <v>0.65</v>
       </c>
-      <c r="G6" s="1">
-        <v>8.91</v>
-      </c>
-      <c r="H6" s="3">
-        <v>144</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="H6">
+        <v>144</v>
+      </c>
+      <c r="I6">
         <v>5.8</v>
       </c>
-      <c r="J6" s="1">
-        <f t="shared" si="0"/>
+      <c r="J6">
         <v>-46.8</v>
       </c>
-      <c r="K6" s="1">
-        <f t="shared" si="1"/>
+      <c r="K6">
         <v>46.8</v>
       </c>
       <c r="L6">
-        <f t="shared" si="2"/>
         <v>-2925</v>
       </c>
       <c r="M6">
-        <f t="shared" si="3"/>
         <v>2925</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6">
+        <v>294.5</v>
+      </c>
+      <c r="O6">
+        <v>306.5</v>
+      </c>
+      <c r="P6">
+        <f>-E6/2*F6</f>
+        <v>-53.46</v>
+      </c>
+      <c r="Q6">
+        <f>E6/2*F6</f>
+        <v>53.46</v>
+      </c>
+      <c r="R6">
+        <f>E6*F6</f>
+        <v>106.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>93.6</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>120.5</v>
       </c>
       <c r="E7">
         <v>16</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
+        <v>7.53</v>
+      </c>
+      <c r="G7">
         <v>0.65</v>
       </c>
-      <c r="G7" s="1">
-        <v>7.53</v>
-      </c>
-      <c r="H7" s="3">
-        <v>144</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="H7">
+        <v>144</v>
+      </c>
+      <c r="I7">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J7" s="1">
-        <f t="shared" si="0"/>
+      <c r="J7">
         <v>-46.8</v>
       </c>
-      <c r="K7" s="1">
-        <f t="shared" si="1"/>
+      <c r="K7">
         <v>46.8</v>
       </c>
       <c r="L7">
-        <f t="shared" si="2"/>
         <v>-2925</v>
       </c>
       <c r="M7">
-        <f t="shared" si="3"/>
         <v>2925</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7">
+        <v>294.5</v>
+      </c>
+      <c r="O7">
+        <v>306.5</v>
+      </c>
+      <c r="P7">
+        <f>Q6</f>
+        <v>53.46</v>
+      </c>
+      <c r="Q7">
+        <f>P7+E7*F7</f>
+        <v>173.94</v>
+      </c>
+      <c r="R7">
+        <f>E7*F7</f>
+        <v>120.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>93.6</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>120.5</v>
       </c>
       <c r="E8">
         <v>16</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
+        <v>7.53</v>
+      </c>
+      <c r="G8">
         <v>0.65</v>
       </c>
-      <c r="G8" s="1">
-        <v>7.53</v>
-      </c>
-      <c r="H8" s="3">
-        <v>144</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="H8">
+        <v>144</v>
+      </c>
+      <c r="I8">
         <v>4.9000000000000004</v>
       </c>
-      <c r="J8" s="1">
-        <f t="shared" si="0"/>
+      <c r="J8">
         <v>-46.8</v>
       </c>
-      <c r="K8" s="1">
-        <f t="shared" si="1"/>
+      <c r="K8">
         <v>46.8</v>
       </c>
       <c r="L8">
-        <f t="shared" si="2"/>
         <v>-2925</v>
       </c>
       <c r="M8">
-        <f t="shared" si="3"/>
         <v>2925</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8">
+        <v>294.5</v>
+      </c>
+      <c r="O8">
+        <v>306.5</v>
+      </c>
+      <c r="P8">
+        <f>Q7</f>
+        <v>173.94</v>
+      </c>
+      <c r="Q8">
+        <f>P8+E8*F8</f>
+        <v>294.42</v>
+      </c>
+      <c r="R8">
+        <f>E8*F8</f>
+        <v>120.48</v>
+      </c>
+      <c r="S8">
+        <f>Q8-P4</f>
+        <v>588.84</v>
+      </c>
+      <c r="T8">
+        <f>SUM(D4:D8)</f>
+        <v>589</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>98.1</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>128</v>
       </c>
       <c r="E9">
         <v>16</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
         <v>0.68</v>
       </c>
-      <c r="G9" s="1">
-        <v>8</v>
-      </c>
-      <c r="H9" s="3">
-        <v>144</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="H9">
+        <v>144</v>
+      </c>
+      <c r="I9">
         <v>5.45</v>
       </c>
-      <c r="J9" s="1">
-        <f t="shared" si="0"/>
+      <c r="J9">
         <v>-49.05</v>
       </c>
-      <c r="K9" s="1">
-        <f t="shared" si="1"/>
+      <c r="K9">
         <v>49.05</v>
       </c>
       <c r="L9">
-        <f t="shared" si="2"/>
         <v>-3065</v>
       </c>
       <c r="M9">
-        <f t="shared" si="3"/>
         <v>3065</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9">
+        <v>307.10000000000002</v>
+      </c>
+      <c r="O9">
+        <v>319.10000000000002</v>
+      </c>
+      <c r="P9">
+        <f>Q9-E9*F9</f>
+        <v>-309.46000000000004</v>
+      </c>
+      <c r="Q9">
+        <f>P10</f>
+        <v>-181.46</v>
+      </c>
+      <c r="R9">
+        <f>E9*F9</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>98.1</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>128</v>
       </c>
       <c r="E10">
         <v>16</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
         <v>0.68</v>
       </c>
-      <c r="G10" s="1">
-        <v>8</v>
-      </c>
-      <c r="H10" s="3">
-        <v>144</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="H10">
+        <v>144</v>
+      </c>
+      <c r="I10">
         <v>5.45</v>
       </c>
-      <c r="J10" s="1">
-        <f t="shared" si="0"/>
+      <c r="J10">
         <v>-49.05</v>
       </c>
-      <c r="K10" s="1">
-        <f t="shared" si="1"/>
+      <c r="K10">
         <v>49.05</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
         <v>-3065</v>
       </c>
       <c r="M10">
-        <f t="shared" si="3"/>
         <v>3065</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N10">
+        <v>307.10000000000002</v>
+      </c>
+      <c r="O10">
+        <v>319.10000000000002</v>
+      </c>
+      <c r="P10">
+        <f>Q10-E10*F10</f>
+        <v>-181.46</v>
+      </c>
+      <c r="Q10">
+        <f>P11</f>
+        <v>-53.46</v>
+      </c>
+      <c r="R10">
+        <f>E10*F10</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>98.1</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>107</v>
       </c>
       <c r="E11">
         <v>12</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11">
+        <v>8.91</v>
+      </c>
+      <c r="G11">
         <v>0.68</v>
       </c>
-      <c r="G11" s="1">
-        <v>8.91</v>
-      </c>
-      <c r="H11" s="3">
-        <v>144</v>
-      </c>
-      <c r="I11" s="1">
+      <c r="H11">
+        <v>144</v>
+      </c>
+      <c r="I11">
         <v>6.07</v>
       </c>
-      <c r="J11" s="1">
-        <f t="shared" si="0"/>
+      <c r="J11">
         <v>-49.05</v>
       </c>
-      <c r="K11" s="1">
-        <f t="shared" si="1"/>
+      <c r="K11">
         <v>49.05</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
         <v>-3065</v>
       </c>
       <c r="M11">
-        <f t="shared" si="3"/>
         <v>3065</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N11">
+        <v>307.10000000000002</v>
+      </c>
+      <c r="O11">
+        <v>319.10000000000002</v>
+      </c>
+      <c r="P11">
+        <f>-E11/2*F11</f>
+        <v>-53.46</v>
+      </c>
+      <c r="Q11">
+        <f>E11/2*F11</f>
+        <v>53.46</v>
+      </c>
+      <c r="R11">
+        <f>E11*F11</f>
+        <v>106.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>98.1</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <v>128</v>
       </c>
       <c r="E12">
         <v>16</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12">
         <v>0.68</v>
       </c>
-      <c r="G12" s="1">
-        <v>8</v>
-      </c>
-      <c r="H12" s="3">
-        <v>144</v>
-      </c>
-      <c r="I12" s="1">
+      <c r="H12">
+        <v>144</v>
+      </c>
+      <c r="I12">
         <v>5.45</v>
       </c>
-      <c r="J12" s="1">
-        <f t="shared" si="0"/>
+      <c r="J12">
         <v>-49.05</v>
       </c>
-      <c r="K12" s="1">
-        <f t="shared" si="1"/>
+      <c r="K12">
         <v>49.05</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
         <v>-3065</v>
       </c>
       <c r="M12">
-        <f t="shared" si="3"/>
         <v>3065</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12">
+        <v>307.10000000000002</v>
+      </c>
+      <c r="O12">
+        <v>319.10000000000002</v>
+      </c>
+      <c r="P12">
+        <f>Q11</f>
+        <v>53.46</v>
+      </c>
+      <c r="Q12">
+        <f>P12+E12*F12</f>
+        <v>181.46</v>
+      </c>
+      <c r="R12">
+        <f>E12*F12</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>98.1</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>128</v>
       </c>
       <c r="E13">
         <v>16</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13">
         <v>0.68</v>
       </c>
-      <c r="G13" s="1">
-        <v>8</v>
-      </c>
-      <c r="H13" s="3">
-        <v>144</v>
-      </c>
-      <c r="I13" s="1">
+      <c r="H13">
+        <v>144</v>
+      </c>
+      <c r="I13">
         <v>5.45</v>
       </c>
-      <c r="J13" s="1">
-        <f t="shared" si="0"/>
+      <c r="J13">
         <v>-49.05</v>
       </c>
-      <c r="K13" s="1">
-        <f t="shared" si="1"/>
+      <c r="K13">
         <v>49.05</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
         <v>-3065</v>
       </c>
       <c r="M13">
-        <f t="shared" si="3"/>
         <v>3065</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N13">
+        <v>307.10000000000002</v>
+      </c>
+      <c r="O13">
+        <v>319.10000000000002</v>
+      </c>
+      <c r="P13">
+        <f>Q12</f>
+        <v>181.46</v>
+      </c>
+      <c r="Q13">
+        <f>P13+E13*F13</f>
+        <v>309.46000000000004</v>
+      </c>
+      <c r="R13">
+        <f>E13*F13</f>
+        <v>128</v>
+      </c>
+      <c r="S13">
+        <f>Q13-P9</f>
+        <v>618.92000000000007</v>
+      </c>
+      <c r="T13">
+        <f>SUM(D9:D13)</f>
+        <v>619</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>102.5</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>131.5</v>
       </c>
       <c r="E14">
         <v>16</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="G14">
         <v>0.71</v>
       </c>
-      <c r="G14" s="1">
-        <v>8.2100000000000009</v>
-      </c>
-      <c r="H14" s="3">
-        <v>144</v>
-      </c>
-      <c r="I14" s="1">
+      <c r="H14">
+        <v>144</v>
+      </c>
+      <c r="I14">
         <v>5.85</v>
       </c>
-      <c r="J14" s="1">
-        <f t="shared" si="0"/>
+      <c r="J14">
         <v>-51.25</v>
       </c>
-      <c r="K14" s="1">
-        <f t="shared" si="1"/>
+      <c r="K14">
         <v>51.25</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
         <v>-3203</v>
       </c>
       <c r="M14">
-        <f t="shared" si="3"/>
         <v>3203</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N14">
+        <v>319.7</v>
+      </c>
+      <c r="O14">
+        <v>331.7</v>
+      </c>
+      <c r="P14">
+        <f>Q14-E14*F14</f>
+        <v>-320.18000000000006</v>
+      </c>
+      <c r="Q14">
+        <f>P15</f>
+        <v>-188.82000000000002</v>
+      </c>
+      <c r="R14">
+        <f>E14*F14</f>
+        <v>131.36000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>102.5</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
         <v>135.5</v>
       </c>
       <c r="E15">
         <v>16</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="G15">
         <v>0.71</v>
       </c>
-      <c r="G15" s="1">
-        <v>8.4600000000000009</v>
-      </c>
-      <c r="H15" s="3">
-        <v>144</v>
-      </c>
-      <c r="I15" s="1">
+      <c r="H15">
+        <v>144</v>
+      </c>
+      <c r="I15">
         <v>6.03</v>
       </c>
-      <c r="J15" s="1">
-        <f t="shared" si="0"/>
+      <c r="J15">
         <v>-51.25</v>
       </c>
-      <c r="K15" s="1">
-        <f t="shared" si="1"/>
+      <c r="K15">
         <v>51.25</v>
       </c>
       <c r="L15">
-        <f t="shared" si="2"/>
         <v>-3203</v>
       </c>
       <c r="M15">
-        <f t="shared" si="3"/>
         <v>3203</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N15">
+        <v>319.7</v>
+      </c>
+      <c r="O15">
+        <v>331.7</v>
+      </c>
+      <c r="P15">
+        <f>Q15-E15*F15</f>
+        <v>-188.82000000000002</v>
+      </c>
+      <c r="Q15">
+        <f>P16</f>
+        <v>-53.46</v>
+      </c>
+      <c r="R15">
+        <f>E15*F15</f>
+        <v>135.36000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>102.5</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
         <v>107</v>
       </c>
       <c r="E16">
         <v>12</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16">
+        <v>8.91</v>
+      </c>
+      <c r="G16">
         <v>0.71</v>
       </c>
-      <c r="G16" s="1">
-        <v>8.91</v>
-      </c>
-      <c r="H16" s="3">
-        <v>144</v>
-      </c>
-      <c r="I16" s="1">
+      <c r="H16">
+        <v>144</v>
+      </c>
+      <c r="I16">
         <v>6.35</v>
       </c>
-      <c r="J16" s="1">
-        <f t="shared" si="0"/>
+      <c r="J16">
         <v>-51.25</v>
       </c>
-      <c r="K16" s="1">
-        <f t="shared" si="1"/>
+      <c r="K16">
         <v>51.25</v>
       </c>
       <c r="L16">
-        <f t="shared" si="2"/>
         <v>-3203</v>
       </c>
       <c r="M16">
-        <f t="shared" si="3"/>
         <v>3203</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N16">
+        <v>319.7</v>
+      </c>
+      <c r="O16">
+        <v>331.7</v>
+      </c>
+      <c r="P16">
+        <f>-E16/2*F16</f>
+        <v>-53.46</v>
+      </c>
+      <c r="Q16">
+        <f>E16/2*F16</f>
+        <v>53.46</v>
+      </c>
+      <c r="R16">
+        <f>E16*F16</f>
+        <v>106.92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>102.5</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17">
         <v>135.5</v>
       </c>
       <c r="E17">
         <v>16</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="G17">
         <v>0.71</v>
       </c>
-      <c r="G17" s="1">
-        <v>8.4600000000000009</v>
-      </c>
-      <c r="H17" s="3">
-        <v>144</v>
-      </c>
-      <c r="I17" s="1">
+      <c r="H17">
+        <v>144</v>
+      </c>
+      <c r="I17">
         <v>6.03</v>
       </c>
-      <c r="J17" s="1">
-        <f t="shared" si="0"/>
+      <c r="J17">
         <v>-51.25</v>
       </c>
-      <c r="K17" s="1">
-        <f t="shared" si="1"/>
+      <c r="K17">
         <v>51.25</v>
       </c>
       <c r="L17">
-        <f t="shared" si="2"/>
         <v>-3203</v>
       </c>
       <c r="M17">
-        <f t="shared" si="3"/>
         <v>3203</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N17">
+        <v>319.7</v>
+      </c>
+      <c r="O17">
+        <v>331.7</v>
+      </c>
+      <c r="P17">
+        <f>Q16</f>
+        <v>53.46</v>
+      </c>
+      <c r="Q17">
+        <f>P17+E17*F17</f>
+        <v>188.82000000000002</v>
+      </c>
+      <c r="R17">
+        <f>E17*F17</f>
+        <v>135.36000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18">
         <v>4</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>102.5</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18">
         <v>131.5</v>
       </c>
       <c r="E18">
         <v>16</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="G18">
         <v>0.71</v>
       </c>
-      <c r="G18" s="1">
-        <v>8.2100000000000009</v>
-      </c>
-      <c r="H18" s="3">
-        <v>144</v>
-      </c>
-      <c r="I18" s="1">
+      <c r="H18">
+        <v>144</v>
+      </c>
+      <c r="I18">
         <v>5.85</v>
       </c>
-      <c r="J18" s="1">
-        <f t="shared" si="0"/>
+      <c r="J18">
         <v>-51.25</v>
       </c>
-      <c r="K18" s="1">
-        <f t="shared" si="1"/>
+      <c r="K18">
         <v>51.25</v>
       </c>
       <c r="L18">
-        <f t="shared" si="2"/>
         <v>-3203</v>
       </c>
       <c r="M18">
-        <f t="shared" si="3"/>
         <v>3203</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N18">
+        <v>319.7</v>
+      </c>
+      <c r="O18">
+        <v>331.7</v>
+      </c>
+      <c r="P18">
+        <f>Q17</f>
+        <v>188.82000000000002</v>
+      </c>
+      <c r="Q18">
+        <f>P18+E18*F18</f>
+        <v>320.18000000000006</v>
+      </c>
+      <c r="R18">
+        <f>E18*F18</f>
+        <v>131.36000000000001</v>
+      </c>
+      <c r="S18">
+        <f>Q18-P14</f>
+        <v>640.36000000000013</v>
+      </c>
+      <c r="T18">
+        <f>SUM(D14:D18)</f>
+        <v>641</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>106.9</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19">
         <v>139</v>
       </c>
       <c r="E19">
         <v>16</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
+        <v>8.68</v>
+      </c>
+      <c r="G19">
         <v>0.74</v>
       </c>
-      <c r="G19" s="1">
-        <v>8.68</v>
-      </c>
-      <c r="H19" s="3">
-        <v>144</v>
-      </c>
-      <c r="I19" s="1">
+      <c r="H19">
+        <v>144</v>
+      </c>
+      <c r="I19">
         <v>6.45</v>
       </c>
-      <c r="J19" s="1">
-        <f t="shared" si="0"/>
+      <c r="J19">
         <v>-53.45</v>
       </c>
-      <c r="K19" s="1">
-        <f t="shared" si="1"/>
+      <c r="K19">
         <v>53.45</v>
       </c>
       <c r="L19">
-        <f t="shared" si="2"/>
         <v>-3340</v>
       </c>
       <c r="M19">
-        <f t="shared" si="3"/>
         <v>3340</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N19">
+        <v>332.3</v>
+      </c>
+      <c r="O19">
+        <v>344.3</v>
+      </c>
+      <c r="P19">
+        <f>Q19-E19*F19</f>
+        <v>-335.22</v>
+      </c>
+      <c r="Q19">
+        <f>P20</f>
+        <v>-196.34</v>
+      </c>
+      <c r="R19">
+        <f>E19*F19</f>
+        <v>138.88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>106.9</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20">
         <v>143</v>
       </c>
       <c r="E20">
         <v>16</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20">
+        <v>8.93</v>
+      </c>
+      <c r="G20">
         <v>0.74</v>
       </c>
-      <c r="G20" s="1">
-        <v>8.93</v>
-      </c>
-      <c r="H20" s="3">
-        <v>144</v>
-      </c>
-      <c r="I20" s="1">
+      <c r="H20">
+        <v>144</v>
+      </c>
+      <c r="I20">
         <v>6.63</v>
       </c>
-      <c r="J20" s="1">
-        <f t="shared" si="0"/>
+      <c r="J20">
         <v>-53.45</v>
       </c>
-      <c r="K20" s="1">
-        <f t="shared" si="1"/>
+      <c r="K20">
         <v>53.45</v>
       </c>
       <c r="L20">
-        <f t="shared" si="2"/>
         <v>-3340</v>
       </c>
       <c r="M20">
-        <f t="shared" si="3"/>
         <v>3340</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N20">
+        <v>332.3</v>
+      </c>
+      <c r="O20">
+        <v>344.3</v>
+      </c>
+      <c r="P20">
+        <f>Q20-E20*F20</f>
+        <v>-196.34</v>
+      </c>
+      <c r="Q20">
+        <f>P21</f>
+        <v>-53.46</v>
+      </c>
+      <c r="R20">
+        <f>E20*F20</f>
+        <v>142.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>106.9</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21">
         <v>107</v>
       </c>
       <c r="E21">
         <v>12</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21">
+        <v>8.91</v>
+      </c>
+      <c r="G21">
         <v>0.74</v>
       </c>
-      <c r="G21" s="1">
-        <v>8.91</v>
-      </c>
-      <c r="H21" s="3">
-        <v>144</v>
-      </c>
-      <c r="I21" s="1">
+      <c r="H21">
+        <v>144</v>
+      </c>
+      <c r="I21">
         <v>6.62</v>
       </c>
-      <c r="J21" s="1">
-        <f t="shared" si="0"/>
+      <c r="J21">
         <v>-53.45</v>
       </c>
-      <c r="K21" s="1">
-        <f t="shared" si="1"/>
+      <c r="K21">
         <v>53.45</v>
       </c>
       <c r="L21">
-        <f t="shared" si="2"/>
         <v>-3340</v>
       </c>
       <c r="M21">
-        <f t="shared" si="3"/>
         <v>3340</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N21">
+        <v>332.3</v>
+      </c>
+      <c r="O21">
+        <v>344.3</v>
+      </c>
+      <c r="P21">
+        <f>-E21/2*F21</f>
+        <v>-53.46</v>
+      </c>
+      <c r="Q21">
+        <f>E21/2*F21</f>
+        <v>53.46</v>
+      </c>
+      <c r="R21">
+        <f>E21*F21</f>
+        <v>106.92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>106.9</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22">
         <v>143</v>
       </c>
       <c r="E22">
         <v>16</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22">
+        <v>8.93</v>
+      </c>
+      <c r="G22">
         <v>0.74</v>
       </c>
-      <c r="G22" s="1">
-        <v>8.93</v>
-      </c>
-      <c r="H22" s="3">
-        <v>144</v>
-      </c>
-      <c r="I22" s="1">
+      <c r="H22">
+        <v>144</v>
+      </c>
+      <c r="I22">
         <v>6.63</v>
       </c>
-      <c r="J22" s="1">
-        <f t="shared" si="0"/>
+      <c r="J22">
         <v>-53.45</v>
       </c>
-      <c r="K22" s="1">
-        <f t="shared" si="1"/>
+      <c r="K22">
         <v>53.45</v>
       </c>
       <c r="L22">
-        <f t="shared" si="2"/>
         <v>-3340</v>
       </c>
       <c r="M22">
-        <f t="shared" si="3"/>
         <v>3340</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N22">
+        <v>332.3</v>
+      </c>
+      <c r="O22">
+        <v>344.3</v>
+      </c>
+      <c r="P22">
+        <f>Q21</f>
+        <v>53.46</v>
+      </c>
+      <c r="Q22">
+        <f>P22+E22*F22</f>
+        <v>196.34</v>
+      </c>
+      <c r="R22">
+        <f>E22*F22</f>
+        <v>142.88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
       <c r="B23">
         <v>4</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
         <v>106.9</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23">
         <v>139</v>
       </c>
       <c r="E23">
         <v>16</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23">
+        <v>8.68</v>
+      </c>
+      <c r="G23">
         <v>0.74</v>
       </c>
-      <c r="G23" s="1">
-        <v>8.68</v>
-      </c>
-      <c r="H23" s="3">
-        <v>144</v>
-      </c>
-      <c r="I23" s="1">
+      <c r="H23">
+        <v>144</v>
+      </c>
+      <c r="I23">
         <v>6.45</v>
       </c>
-      <c r="J23" s="1">
-        <f t="shared" si="0"/>
+      <c r="J23">
         <v>-53.45</v>
       </c>
-      <c r="K23" s="1">
-        <f t="shared" si="1"/>
+      <c r="K23">
         <v>53.45</v>
       </c>
       <c r="L23">
-        <f t="shared" si="2"/>
         <v>-3340</v>
       </c>
       <c r="M23">
-        <f t="shared" si="3"/>
         <v>3340</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N23">
+        <v>332.3</v>
+      </c>
+      <c r="O23">
+        <v>344.3</v>
+      </c>
+      <c r="P23">
+        <f>Q22</f>
+        <v>196.34</v>
+      </c>
+      <c r="Q23">
+        <f>P23+E23*F23</f>
+        <v>335.22</v>
+      </c>
+      <c r="R23">
+        <f>E23*F23</f>
+        <v>138.88</v>
+      </c>
+      <c r="S23">
+        <f>Q23-P19</f>
+        <v>670.44</v>
+      </c>
+      <c r="T23">
+        <f>SUM(D19:D23)</f>
+        <v>671</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
         <v>111.4</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24">
         <v>139</v>
       </c>
       <c r="E24">
         <v>14</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24">
+        <v>9.92</v>
+      </c>
+      <c r="G24">
         <v>0.77</v>
       </c>
-      <c r="G24" s="1">
-        <v>9.92</v>
-      </c>
-      <c r="H24" s="3">
-        <v>144</v>
-      </c>
-      <c r="I24" s="1">
+      <c r="H24">
+        <v>144</v>
+      </c>
+      <c r="I24">
         <v>7.68</v>
       </c>
-      <c r="J24" s="1">
-        <f t="shared" si="0"/>
+      <c r="J24">
         <v>-55.7</v>
       </c>
-      <c r="K24" s="1">
-        <f t="shared" si="1"/>
+      <c r="K24">
         <v>55.7</v>
       </c>
       <c r="L24">
-        <f t="shared" si="2"/>
         <v>-3481</v>
       </c>
       <c r="M24">
-        <f t="shared" si="3"/>
         <v>3481</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N24">
+        <v>344.9</v>
+      </c>
+      <c r="O24">
+        <v>356.9</v>
+      </c>
+      <c r="P24">
+        <f>Q24-E24*F24</f>
+        <v>-342.26</v>
+      </c>
+      <c r="Q24">
+        <f>P25</f>
+        <v>-203.38</v>
+      </c>
+      <c r="R24">
+        <f>E24*F24</f>
+        <v>138.88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25">
         <v>111.4</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25">
         <v>150</v>
       </c>
       <c r="E25">
         <v>16</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="G25">
         <v>0.77</v>
       </c>
-      <c r="G25" s="1">
-        <v>9.3699999999999992</v>
-      </c>
-      <c r="H25" s="3">
-        <v>144</v>
-      </c>
-      <c r="I25" s="1">
+      <c r="H25">
+        <v>144</v>
+      </c>
+      <c r="I25">
         <v>7.25</v>
       </c>
-      <c r="J25" s="1">
-        <f t="shared" si="0"/>
+      <c r="J25">
         <v>-55.7</v>
       </c>
-      <c r="K25" s="1">
-        <f t="shared" si="1"/>
+      <c r="K25">
         <v>55.7</v>
       </c>
       <c r="L25">
-        <f t="shared" si="2"/>
         <v>-3481</v>
       </c>
       <c r="M25">
-        <f t="shared" si="3"/>
         <v>3481</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N25">
+        <v>344.9</v>
+      </c>
+      <c r="O25">
+        <v>356.9</v>
+      </c>
+      <c r="P25">
+        <f>Q25-E25*F25</f>
+        <v>-203.38</v>
+      </c>
+      <c r="Q25">
+        <f>P26</f>
+        <v>-53.46</v>
+      </c>
+      <c r="R25">
+        <f>E25*F25</f>
+        <v>149.91999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26">
         <v>111.4</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26">
         <v>107</v>
       </c>
       <c r="E26">
         <v>12</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26">
+        <v>8.91</v>
+      </c>
+      <c r="G26">
         <v>0.77</v>
       </c>
-      <c r="G26" s="1">
-        <v>8.91</v>
-      </c>
-      <c r="H26" s="3">
-        <v>144</v>
-      </c>
-      <c r="I26" s="1">
+      <c r="H26">
+        <v>144</v>
+      </c>
+      <c r="I26">
         <v>6.9</v>
       </c>
-      <c r="J26" s="1">
-        <f t="shared" si="0"/>
+      <c r="J26">
         <v>-55.7</v>
       </c>
-      <c r="K26" s="1">
-        <f t="shared" si="1"/>
+      <c r="K26">
         <v>55.7</v>
       </c>
       <c r="L26">
-        <f t="shared" si="2"/>
         <v>-3481</v>
       </c>
       <c r="M26">
-        <f t="shared" si="3"/>
         <v>3481</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N26">
+        <v>344.9</v>
+      </c>
+      <c r="O26">
+        <v>356.9</v>
+      </c>
+      <c r="P26">
+        <f>-E26/2*F26</f>
+        <v>-53.46</v>
+      </c>
+      <c r="Q26">
+        <f>E26/2*F26</f>
+        <v>53.46</v>
+      </c>
+      <c r="R26">
+        <f>E26*F26</f>
+        <v>106.92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>111.4</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27">
         <v>150</v>
       </c>
       <c r="E27">
         <v>16</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="G27">
         <v>0.77</v>
       </c>
-      <c r="G27" s="1">
-        <v>9.3699999999999992</v>
-      </c>
-      <c r="H27" s="3">
-        <v>144</v>
-      </c>
-      <c r="I27" s="1">
+      <c r="H27">
+        <v>144</v>
+      </c>
+      <c r="I27">
         <v>7.25</v>
       </c>
-      <c r="J27" s="1">
-        <f t="shared" si="0"/>
+      <c r="J27">
         <v>-55.7</v>
       </c>
-      <c r="K27" s="1">
-        <f t="shared" si="1"/>
+      <c r="K27">
         <v>55.7</v>
       </c>
       <c r="L27">
-        <f t="shared" si="2"/>
         <v>-3481</v>
       </c>
       <c r="M27">
-        <f t="shared" si="3"/>
         <v>3481</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N27">
+        <v>344.9</v>
+      </c>
+      <c r="O27">
+        <v>356.9</v>
+      </c>
+      <c r="P27">
+        <f>Q26</f>
+        <v>53.46</v>
+      </c>
+      <c r="Q27">
+        <f>P27+E27*F27</f>
+        <v>203.38</v>
+      </c>
+      <c r="R27">
+        <f>E27*F27</f>
+        <v>149.91999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
       <c r="B28">
         <v>4</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28">
         <v>111.4</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28">
         <v>139</v>
       </c>
       <c r="E28">
         <v>14</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28">
+        <v>9.92</v>
+      </c>
+      <c r="G28">
         <v>0.77</v>
       </c>
-      <c r="G28" s="1">
-        <v>9.92</v>
-      </c>
-      <c r="H28" s="3">
-        <v>144</v>
-      </c>
-      <c r="I28" s="1">
+      <c r="H28">
+        <v>144</v>
+      </c>
+      <c r="I28">
         <v>7.68</v>
       </c>
-      <c r="J28" s="1">
-        <f t="shared" si="0"/>
+      <c r="J28">
         <v>-55.7</v>
       </c>
-      <c r="K28" s="1">
-        <f t="shared" si="1"/>
+      <c r="K28">
         <v>55.7</v>
       </c>
       <c r="L28">
-        <f t="shared" si="2"/>
         <v>-3481</v>
       </c>
       <c r="M28">
-        <f t="shared" si="3"/>
         <v>3481</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N28">
+        <v>344.9</v>
+      </c>
+      <c r="O28">
+        <v>356.9</v>
+      </c>
+      <c r="P28">
+        <f>Q27</f>
+        <v>203.38</v>
+      </c>
+      <c r="Q28">
+        <f>P28+E28*F28</f>
+        <v>342.26</v>
+      </c>
+      <c r="R28">
+        <f>E28*F28</f>
+        <v>138.88</v>
+      </c>
+      <c r="S28">
+        <f>Q28-P24</f>
+        <v>684.52</v>
+      </c>
+      <c r="T28">
+        <f>SUM(D24:D28)</f>
+        <v>685</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29">
         <v>115.8</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29">
         <v>131.5</v>
       </c>
       <c r="E29">
         <v>13</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29">
+        <v>10.11</v>
+      </c>
+      <c r="G29">
         <v>0.8</v>
       </c>
-      <c r="G29" s="1">
-        <v>10.11</v>
-      </c>
-      <c r="H29" s="3">
-        <v>144</v>
-      </c>
-      <c r="I29" s="1">
+      <c r="H29">
+        <v>144</v>
+      </c>
+      <c r="I29">
         <v>8.1300000000000008</v>
       </c>
-      <c r="J29" s="1">
-        <f t="shared" si="0"/>
+      <c r="J29">
         <v>-57.9</v>
       </c>
-      <c r="K29" s="1">
-        <f t="shared" si="1"/>
+      <c r="K29">
         <v>57.9</v>
       </c>
       <c r="L29">
-        <f t="shared" si="2"/>
         <v>-3618</v>
       </c>
       <c r="M29">
-        <f t="shared" si="3"/>
         <v>3618</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N29">
+        <v>357.5</v>
+      </c>
+      <c r="O29">
+        <v>369.5</v>
+      </c>
+      <c r="P29">
+        <f>Q29-E29*F29</f>
+        <v>-342.33000000000004</v>
+      </c>
+      <c r="Q29">
+        <f>P30</f>
+        <v>-210.9</v>
+      </c>
+      <c r="R29">
+        <f>E29*F29</f>
+        <v>131.43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30">
         <v>115.8</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30">
         <v>157.5</v>
       </c>
       <c r="E30">
         <v>16</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30">
+        <v>9.84</v>
+      </c>
+      <c r="G30">
         <v>0.8</v>
       </c>
-      <c r="G30" s="1">
-        <v>9.84</v>
-      </c>
-      <c r="H30" s="3">
-        <v>144</v>
-      </c>
-      <c r="I30" s="1">
+      <c r="H30">
+        <v>144</v>
+      </c>
+      <c r="I30">
         <v>7.92</v>
       </c>
-      <c r="J30" s="1">
-        <f t="shared" si="0"/>
+      <c r="J30">
         <v>-57.9</v>
       </c>
-      <c r="K30" s="1">
-        <f t="shared" si="1"/>
+      <c r="K30">
         <v>57.9</v>
       </c>
       <c r="L30">
-        <f t="shared" si="2"/>
         <v>-3618</v>
       </c>
       <c r="M30">
-        <f t="shared" si="3"/>
         <v>3618</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N30">
+        <v>357.5</v>
+      </c>
+      <c r="O30">
+        <v>369.5</v>
+      </c>
+      <c r="P30">
+        <f>Q30-E30*F30</f>
+        <v>-210.9</v>
+      </c>
+      <c r="Q30">
+        <f>P31</f>
+        <v>-53.46</v>
+      </c>
+      <c r="R30">
+        <f>E30*F30</f>
+        <v>157.44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>5</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31">
         <v>115.8</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31">
         <v>107</v>
       </c>
       <c r="E31">
         <v>12</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31">
+        <v>8.91</v>
+      </c>
+      <c r="G31">
         <v>0.8</v>
       </c>
-      <c r="G31" s="1">
-        <v>8.91</v>
-      </c>
-      <c r="H31" s="3">
-        <v>144</v>
-      </c>
-      <c r="I31" s="1">
+      <c r="H31">
+        <v>144</v>
+      </c>
+      <c r="I31">
         <v>7.17</v>
       </c>
-      <c r="J31" s="1">
-        <f t="shared" si="0"/>
+      <c r="J31">
         <v>-57.9</v>
       </c>
-      <c r="K31" s="1">
-        <f t="shared" si="1"/>
+      <c r="K31">
         <v>57.9</v>
       </c>
       <c r="L31">
-        <f t="shared" si="2"/>
         <v>-3618</v>
       </c>
       <c r="M31">
-        <f t="shared" si="3"/>
         <v>3618</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N31">
+        <v>357.5</v>
+      </c>
+      <c r="O31">
+        <v>369.5</v>
+      </c>
+      <c r="P31">
+        <f>-E31/2*F31</f>
+        <v>-53.46</v>
+      </c>
+      <c r="Q31">
+        <f>E31/2*F31</f>
+        <v>53.46</v>
+      </c>
+      <c r="R31">
+        <f>E31*F31</f>
+        <v>106.92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>5</v>
       </c>
       <c r="B32">
         <v>3</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32">
         <v>115.8</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32">
         <v>157.5</v>
       </c>
       <c r="E32">
         <v>16</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32">
+        <v>9.84</v>
+      </c>
+      <c r="G32">
         <v>0.8</v>
       </c>
-      <c r="G32" s="1">
-        <v>9.84</v>
-      </c>
-      <c r="H32" s="3">
-        <v>144</v>
-      </c>
-      <c r="I32" s="1">
+      <c r="H32">
+        <v>144</v>
+      </c>
+      <c r="I32">
         <v>7.92</v>
       </c>
-      <c r="J32" s="1">
-        <f t="shared" si="0"/>
+      <c r="J32">
         <v>-57.9</v>
       </c>
-      <c r="K32" s="1">
-        <f t="shared" si="1"/>
+      <c r="K32">
         <v>57.9</v>
       </c>
       <c r="L32">
-        <f t="shared" si="2"/>
         <v>-3618</v>
       </c>
       <c r="M32">
-        <f t="shared" si="3"/>
         <v>3618</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N32">
+        <v>357.5</v>
+      </c>
+      <c r="O32">
+        <v>369.5</v>
+      </c>
+      <c r="P32">
+        <f>Q31</f>
+        <v>53.46</v>
+      </c>
+      <c r="Q32">
+        <f>P32+E32*F32</f>
+        <v>210.9</v>
+      </c>
+      <c r="R32">
+        <f>E32*F32</f>
+        <v>157.44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>5</v>
       </c>
       <c r="B33">
         <v>4</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33">
         <v>115.8</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33">
         <v>131.5</v>
       </c>
       <c r="E33">
         <v>13</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33">
+        <v>10.11</v>
+      </c>
+      <c r="G33">
         <v>0.8</v>
       </c>
-      <c r="G33" s="1">
-        <v>10.11</v>
-      </c>
-      <c r="H33" s="3">
-        <v>144</v>
-      </c>
-      <c r="I33" s="1">
+      <c r="H33">
+        <v>144</v>
+      </c>
+      <c r="I33">
         <v>8.1300000000000008</v>
       </c>
-      <c r="J33" s="1">
-        <f t="shared" si="0"/>
+      <c r="J33">
         <v>-57.9</v>
       </c>
-      <c r="K33" s="1">
-        <f t="shared" si="1"/>
+      <c r="K33">
         <v>57.9</v>
       </c>
       <c r="L33">
-        <f t="shared" si="2"/>
         <v>-3618</v>
       </c>
       <c r="M33">
-        <f t="shared" si="3"/>
         <v>3618</v>
+      </c>
+      <c r="N33">
+        <v>357.5</v>
+      </c>
+      <c r="O33">
+        <v>369.5</v>
+      </c>
+      <c r="P33">
+        <f>Q32</f>
+        <v>210.9</v>
+      </c>
+      <c r="Q33">
+        <f>P33+E33*F33</f>
+        <v>342.33000000000004</v>
+      </c>
+      <c r="R33">
+        <f>E33*F33</f>
+        <v>131.43</v>
+      </c>
+      <c r="S33">
+        <f>Q33-P29</f>
+        <v>684.66000000000008</v>
+      </c>
+      <c r="T33">
+        <f>SUM(D29:D33)</f>
+        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -1978,13 +2456,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2001,10 +2481,10 @@
         <v>11</v>
       </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -2022,7 +2502,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2060,18 +2540,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -2106,8 +2586,17 @@
       <c r="O3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2124,10 +2613,10 @@
         <v>16</v>
       </c>
       <c r="F4">
+        <v>7.53</v>
+      </c>
+      <c r="G4">
         <v>0.65</v>
-      </c>
-      <c r="G4">
-        <v>7.53</v>
       </c>
       <c r="H4">
         <v>144</v>
@@ -2153,8 +2642,17 @@
       <c r="O4">
         <v>306.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <v>-294.42</v>
+      </c>
+      <c r="Q4">
+        <v>-173.94</v>
+      </c>
+      <c r="R4">
+        <v>120.48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2171,10 +2669,10 @@
         <v>16</v>
       </c>
       <c r="F5">
+        <v>7.53</v>
+      </c>
+      <c r="G5">
         <v>0.65</v>
-      </c>
-      <c r="G5">
-        <v>7.53</v>
       </c>
       <c r="H5">
         <v>144</v>
@@ -2200,8 +2698,17 @@
       <c r="O5">
         <v>306.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P5">
+        <v>-173.94</v>
+      </c>
+      <c r="Q5">
+        <v>-53.46</v>
+      </c>
+      <c r="R5">
+        <v>120.48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2218,10 +2725,10 @@
         <v>12</v>
       </c>
       <c r="F6">
+        <v>8.91</v>
+      </c>
+      <c r="G6">
         <v>0.65</v>
-      </c>
-      <c r="G6">
-        <v>8.91</v>
       </c>
       <c r="H6">
         <v>144</v>
@@ -2247,8 +2754,17 @@
       <c r="O6">
         <v>306.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <v>-53.46</v>
+      </c>
+      <c r="Q6">
+        <v>53.46</v>
+      </c>
+      <c r="R6">
+        <v>106.92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2265,10 +2781,10 @@
         <v>16</v>
       </c>
       <c r="F7">
+        <v>7.53</v>
+      </c>
+      <c r="G7">
         <v>0.65</v>
-      </c>
-      <c r="G7">
-        <v>7.53</v>
       </c>
       <c r="H7">
         <v>144</v>
@@ -2294,8 +2810,17 @@
       <c r="O7">
         <v>306.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <v>53.46</v>
+      </c>
+      <c r="Q7">
+        <v>173.94</v>
+      </c>
+      <c r="R7">
+        <v>120.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2312,10 +2837,10 @@
         <v>16</v>
       </c>
       <c r="F8">
+        <v>7.53</v>
+      </c>
+      <c r="G8">
         <v>0.65</v>
-      </c>
-      <c r="G8">
-        <v>7.53</v>
       </c>
       <c r="H8">
         <v>144</v>
@@ -2341,8 +2866,17 @@
       <c r="O8">
         <v>306.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <v>173.94</v>
+      </c>
+      <c r="Q8">
+        <v>294.42</v>
+      </c>
+      <c r="R8">
+        <v>120.48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2359,10 +2893,10 @@
         <v>16</v>
       </c>
       <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
         <v>0.68</v>
-      </c>
-      <c r="G9">
-        <v>8</v>
       </c>
       <c r="H9">
         <v>144</v>
@@ -2388,8 +2922,17 @@
       <c r="O9">
         <v>319.10000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9">
+        <v>-309.46000000000004</v>
+      </c>
+      <c r="Q9">
+        <v>-181.46</v>
+      </c>
+      <c r="R9">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2406,10 +2949,10 @@
         <v>16</v>
       </c>
       <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
         <v>0.68</v>
-      </c>
-      <c r="G10">
-        <v>8</v>
       </c>
       <c r="H10">
         <v>144</v>
@@ -2435,8 +2978,17 @@
       <c r="O10">
         <v>319.10000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10">
+        <v>-181.46</v>
+      </c>
+      <c r="Q10">
+        <v>-53.46</v>
+      </c>
+      <c r="R10">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2453,10 +3005,10 @@
         <v>12</v>
       </c>
       <c r="F11">
+        <v>8.91</v>
+      </c>
+      <c r="G11">
         <v>0.68</v>
-      </c>
-      <c r="G11">
-        <v>8.91</v>
       </c>
       <c r="H11">
         <v>144</v>
@@ -2482,8 +3034,17 @@
       <c r="O11">
         <v>319.10000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11">
+        <v>-53.46</v>
+      </c>
+      <c r="Q11">
+        <v>53.46</v>
+      </c>
+      <c r="R11">
+        <v>106.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2500,10 +3061,10 @@
         <v>16</v>
       </c>
       <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12">
         <v>0.68</v>
-      </c>
-      <c r="G12">
-        <v>8</v>
       </c>
       <c r="H12">
         <v>144</v>
@@ -2529,8 +3090,17 @@
       <c r="O12">
         <v>319.10000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <v>53.46</v>
+      </c>
+      <c r="Q12">
+        <v>181.46</v>
+      </c>
+      <c r="R12">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2547,10 +3117,10 @@
         <v>16</v>
       </c>
       <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13">
         <v>0.68</v>
-      </c>
-      <c r="G13">
-        <v>8</v>
       </c>
       <c r="H13">
         <v>144</v>
@@ -2576,8 +3146,17 @@
       <c r="O13">
         <v>319.10000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13">
+        <v>181.46</v>
+      </c>
+      <c r="Q13">
+        <v>309.46000000000004</v>
+      </c>
+      <c r="R13">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2594,10 +3173,10 @@
         <v>16</v>
       </c>
       <c r="F14">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="G14">
         <v>0.71</v>
-      </c>
-      <c r="G14">
-        <v>8.2100000000000009</v>
       </c>
       <c r="H14">
         <v>144</v>
@@ -2623,8 +3202,17 @@
       <c r="O14">
         <v>331.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14">
+        <v>-320.18000000000006</v>
+      </c>
+      <c r="Q14">
+        <v>-188.82000000000002</v>
+      </c>
+      <c r="R14">
+        <v>131.36000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2641,10 +3229,10 @@
         <v>16</v>
       </c>
       <c r="F15">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="G15">
         <v>0.71</v>
-      </c>
-      <c r="G15">
-        <v>8.4600000000000009</v>
       </c>
       <c r="H15">
         <v>144</v>
@@ -2670,8 +3258,17 @@
       <c r="O15">
         <v>331.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P15">
+        <v>-188.82000000000002</v>
+      </c>
+      <c r="Q15">
+        <v>-53.46</v>
+      </c>
+      <c r="R15">
+        <v>135.36000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2688,10 +3285,10 @@
         <v>12</v>
       </c>
       <c r="F16">
+        <v>8.91</v>
+      </c>
+      <c r="G16">
         <v>0.71</v>
-      </c>
-      <c r="G16">
-        <v>8.91</v>
       </c>
       <c r="H16">
         <v>144</v>
@@ -2717,8 +3314,17 @@
       <c r="O16">
         <v>331.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <v>-53.46</v>
+      </c>
+      <c r="Q16">
+        <v>53.46</v>
+      </c>
+      <c r="R16">
+        <v>106.92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2735,10 +3341,10 @@
         <v>16</v>
       </c>
       <c r="F17">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="G17">
         <v>0.71</v>
-      </c>
-      <c r="G17">
-        <v>8.4600000000000009</v>
       </c>
       <c r="H17">
         <v>144</v>
@@ -2764,8 +3370,17 @@
       <c r="O17">
         <v>331.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <v>53.46</v>
+      </c>
+      <c r="Q17">
+        <v>188.82000000000002</v>
+      </c>
+      <c r="R17">
+        <v>135.36000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2782,10 +3397,10 @@
         <v>16</v>
       </c>
       <c r="F18">
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="G18">
         <v>0.71</v>
-      </c>
-      <c r="G18">
-        <v>8.2100000000000009</v>
       </c>
       <c r="H18">
         <v>144</v>
@@ -2811,8 +3426,17 @@
       <c r="O18">
         <v>331.7</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18">
+        <v>188.82000000000002</v>
+      </c>
+      <c r="Q18">
+        <v>320.18000000000006</v>
+      </c>
+      <c r="R18">
+        <v>131.36000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2829,10 +3453,10 @@
         <v>16</v>
       </c>
       <c r="F19">
+        <v>8.68</v>
+      </c>
+      <c r="G19">
         <v>0.74</v>
-      </c>
-      <c r="G19">
-        <v>8.68</v>
       </c>
       <c r="H19">
         <v>144</v>
@@ -2858,8 +3482,17 @@
       <c r="O19">
         <v>344.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <v>-335.22</v>
+      </c>
+      <c r="Q19">
+        <v>-196.34</v>
+      </c>
+      <c r="R19">
+        <v>138.88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2876,10 +3509,10 @@
         <v>16</v>
       </c>
       <c r="F20">
+        <v>8.93</v>
+      </c>
+      <c r="G20">
         <v>0.74</v>
-      </c>
-      <c r="G20">
-        <v>8.93</v>
       </c>
       <c r="H20">
         <v>144</v>
@@ -2905,8 +3538,17 @@
       <c r="O20">
         <v>344.3</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20">
+        <v>-196.34</v>
+      </c>
+      <c r="Q20">
+        <v>-53.46</v>
+      </c>
+      <c r="R20">
+        <v>142.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2923,10 +3565,10 @@
         <v>12</v>
       </c>
       <c r="F21">
+        <v>8.91</v>
+      </c>
+      <c r="G21">
         <v>0.74</v>
-      </c>
-      <c r="G21">
-        <v>8.91</v>
       </c>
       <c r="H21">
         <v>144</v>
@@ -2952,8 +3594,17 @@
       <c r="O21">
         <v>344.3</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21">
+        <v>-53.46</v>
+      </c>
+      <c r="Q21">
+        <v>53.46</v>
+      </c>
+      <c r="R21">
+        <v>106.92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2970,10 +3621,10 @@
         <v>16</v>
       </c>
       <c r="F22">
+        <v>8.93</v>
+      </c>
+      <c r="G22">
         <v>0.74</v>
-      </c>
-      <c r="G22">
-        <v>8.93</v>
       </c>
       <c r="H22">
         <v>144</v>
@@ -2999,8 +3650,17 @@
       <c r="O22">
         <v>344.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22">
+        <v>53.46</v>
+      </c>
+      <c r="Q22">
+        <v>196.34</v>
+      </c>
+      <c r="R22">
+        <v>142.88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -3017,10 +3677,10 @@
         <v>16</v>
       </c>
       <c r="F23">
+        <v>8.68</v>
+      </c>
+      <c r="G23">
         <v>0.74</v>
-      </c>
-      <c r="G23">
-        <v>8.68</v>
       </c>
       <c r="H23">
         <v>144</v>
@@ -3046,8 +3706,17 @@
       <c r="O23">
         <v>344.3</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23">
+        <v>196.34</v>
+      </c>
+      <c r="Q23">
+        <v>335.22</v>
+      </c>
+      <c r="R23">
+        <v>138.88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
@@ -3064,10 +3733,10 @@
         <v>14</v>
       </c>
       <c r="F24">
+        <v>9.92</v>
+      </c>
+      <c r="G24">
         <v>0.77</v>
-      </c>
-      <c r="G24">
-        <v>9.92</v>
       </c>
       <c r="H24">
         <v>144</v>
@@ -3093,8 +3762,17 @@
       <c r="O24">
         <v>356.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24">
+        <v>-342.26</v>
+      </c>
+      <c r="Q24">
+        <v>-203.38</v>
+      </c>
+      <c r="R24">
+        <v>138.88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
@@ -3111,10 +3789,10 @@
         <v>16</v>
       </c>
       <c r="F25">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="G25">
         <v>0.77</v>
-      </c>
-      <c r="G25">
-        <v>9.3699999999999992</v>
       </c>
       <c r="H25">
         <v>144</v>
@@ -3140,8 +3818,17 @@
       <c r="O25">
         <v>356.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25">
+        <v>-203.38</v>
+      </c>
+      <c r="Q25">
+        <v>-53.46</v>
+      </c>
+      <c r="R25">
+        <v>149.91999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
@@ -3158,10 +3845,10 @@
         <v>12</v>
       </c>
       <c r="F26">
+        <v>8.91</v>
+      </c>
+      <c r="G26">
         <v>0.77</v>
-      </c>
-      <c r="G26">
-        <v>8.91</v>
       </c>
       <c r="H26">
         <v>144</v>
@@ -3187,8 +3874,17 @@
       <c r="O26">
         <v>356.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26">
+        <v>-53.46</v>
+      </c>
+      <c r="Q26">
+        <v>53.46</v>
+      </c>
+      <c r="R26">
+        <v>106.92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4</v>
       </c>
@@ -3205,10 +3901,10 @@
         <v>16</v>
       </c>
       <c r="F27">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="G27">
         <v>0.77</v>
-      </c>
-      <c r="G27">
-        <v>9.3699999999999992</v>
       </c>
       <c r="H27">
         <v>144</v>
@@ -3234,8 +3930,17 @@
       <c r="O27">
         <v>356.9</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27">
+        <v>53.46</v>
+      </c>
+      <c r="Q27">
+        <v>203.38</v>
+      </c>
+      <c r="R27">
+        <v>149.91999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4</v>
       </c>
@@ -3252,10 +3957,10 @@
         <v>14</v>
       </c>
       <c r="F28">
+        <v>9.92</v>
+      </c>
+      <c r="G28">
         <v>0.77</v>
-      </c>
-      <c r="G28">
-        <v>9.92</v>
       </c>
       <c r="H28">
         <v>144</v>
@@ -3281,8 +3986,17 @@
       <c r="O28">
         <v>356.9</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P28">
+        <v>203.38</v>
+      </c>
+      <c r="Q28">
+        <v>342.26</v>
+      </c>
+      <c r="R28">
+        <v>138.88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
@@ -3299,10 +4013,10 @@
         <v>13</v>
       </c>
       <c r="F29">
+        <v>10.11</v>
+      </c>
+      <c r="G29">
         <v>0.8</v>
-      </c>
-      <c r="G29">
-        <v>10.11</v>
       </c>
       <c r="H29">
         <v>144</v>
@@ -3328,8 +4042,17 @@
       <c r="O29">
         <v>369.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P29">
+        <v>-342.33000000000004</v>
+      </c>
+      <c r="Q29">
+        <v>-210.9</v>
+      </c>
+      <c r="R29">
+        <v>131.43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5</v>
       </c>
@@ -3346,10 +4069,10 @@
         <v>16</v>
       </c>
       <c r="F30">
+        <v>9.84</v>
+      </c>
+      <c r="G30">
         <v>0.8</v>
-      </c>
-      <c r="G30">
-        <v>9.84</v>
       </c>
       <c r="H30">
         <v>144</v>
@@ -3375,8 +4098,17 @@
       <c r="O30">
         <v>369.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P30">
+        <v>-210.9</v>
+      </c>
+      <c r="Q30">
+        <v>-53.46</v>
+      </c>
+      <c r="R30">
+        <v>157.44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>5</v>
       </c>
@@ -3393,10 +4125,10 @@
         <v>12</v>
       </c>
       <c r="F31">
+        <v>8.91</v>
+      </c>
+      <c r="G31">
         <v>0.8</v>
-      </c>
-      <c r="G31">
-        <v>8.91</v>
       </c>
       <c r="H31">
         <v>144</v>
@@ -3422,8 +4154,17 @@
       <c r="O31">
         <v>369.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P31">
+        <v>-53.46</v>
+      </c>
+      <c r="Q31">
+        <v>53.46</v>
+      </c>
+      <c r="R31">
+        <v>106.92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>5</v>
       </c>
@@ -3440,10 +4181,10 @@
         <v>16</v>
       </c>
       <c r="F32">
+        <v>9.84</v>
+      </c>
+      <c r="G32">
         <v>0.8</v>
-      </c>
-      <c r="G32">
-        <v>9.84</v>
       </c>
       <c r="H32">
         <v>144</v>
@@ -3469,8 +4210,17 @@
       <c r="O32">
         <v>369.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P32">
+        <v>53.46</v>
+      </c>
+      <c r="Q32">
+        <v>210.9</v>
+      </c>
+      <c r="R32">
+        <v>157.44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>5</v>
       </c>
@@ -3487,10 +4237,10 @@
         <v>13</v>
       </c>
       <c r="F33">
+        <v>10.11</v>
+      </c>
+      <c r="G33">
         <v>0.8</v>
-      </c>
-      <c r="G33">
-        <v>10.11</v>
       </c>
       <c r="H33">
         <v>144</v>
@@ -3515,6 +4265,15 @@
       </c>
       <c r="O33">
         <v>369.5</v>
+      </c>
+      <c r="P33">
+        <v>210.9</v>
+      </c>
+      <c r="Q33">
+        <v>342.33000000000004</v>
+      </c>
+      <c r="R33">
+        <v>131.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix 13 and 14 row data
</commit_message>
<xml_diff>
--- a/TRDDimensions.xlsx
+++ b/TRDDimensions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\alice\jsroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFC2F79-5EA7-4361-8276-9F7E3A9033ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E85EFB7-A816-47BE-BB83-F67743B15A4E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35505" yWindow="-3510" windowWidth="20865" windowHeight="12795" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:S33"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S33" sqref="A4:S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1940,7 +1940,7 @@
         <v>139</v>
       </c>
       <c r="E24">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F24">
         <v>9.92</v>
@@ -1978,7 +1978,7 @@
       </c>
       <c r="Q24">
         <f>R24-E24*F24</f>
-        <v>-342.26</v>
+        <v>-362.1</v>
       </c>
       <c r="R24">
         <f>Q25</f>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="S24">
         <f t="shared" si="0"/>
-        <v>138.88</v>
+        <v>158.72</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -2192,7 +2192,7 @@
         <v>139</v>
       </c>
       <c r="E28">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F28">
         <v>9.92</v>
@@ -2234,15 +2234,15 @@
       </c>
       <c r="R28">
         <f>Q28+E28*F28</f>
-        <v>342.26</v>
+        <v>362.1</v>
       </c>
       <c r="S28">
         <f t="shared" si="0"/>
-        <v>138.88</v>
+        <v>158.72</v>
       </c>
       <c r="T28">
         <f>R28-Q24</f>
-        <v>684.52</v>
+        <v>724.2</v>
       </c>
       <c r="U28">
         <f>SUM(D24:D28)</f>
@@ -2263,7 +2263,7 @@
         <v>131.5</v>
       </c>
       <c r="E29">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F29">
         <v>10.11</v>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="Q29">
         <f>R29-E29*F29</f>
-        <v>-342.33000000000004</v>
+        <v>-372.65999999999997</v>
       </c>
       <c r="R29">
         <f>Q30</f>
@@ -2309,7 +2309,7 @@
       </c>
       <c r="S29">
         <f t="shared" si="0"/>
-        <v>131.43</v>
+        <v>161.76</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.3">
@@ -2515,7 +2515,7 @@
         <v>131.5</v>
       </c>
       <c r="E33">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F33">
         <v>10.11</v>
@@ -2557,15 +2557,15 @@
       </c>
       <c r="R33">
         <f>Q33+E33*F33</f>
-        <v>342.33000000000004</v>
+        <v>372.65999999999997</v>
       </c>
       <c r="S33">
         <f t="shared" si="0"/>
-        <v>131.43</v>
+        <v>161.76</v>
       </c>
       <c r="T33">
         <f>R33-Q29</f>
-        <v>684.66000000000008</v>
+        <v>745.31999999999994</v>
       </c>
       <c r="U33">
         <f>SUM(D29:D33)</f>
@@ -2587,8 +2587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:S33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3922,7 +3922,7 @@
         <v>139</v>
       </c>
       <c r="E24">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F24">
         <v>9.92</v>
@@ -3958,13 +3958,13 @@
         <v>350.9</v>
       </c>
       <c r="Q24">
-        <v>-342.26</v>
+        <v>-362.1</v>
       </c>
       <c r="R24">
         <v>-203.38</v>
       </c>
       <c r="S24">
-        <v>138.88</v>
+        <v>158.72</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
@@ -4158,7 +4158,7 @@
         <v>139</v>
       </c>
       <c r="E28">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F28">
         <v>9.92</v>
@@ -4197,10 +4197,10 @@
         <v>203.38</v>
       </c>
       <c r="R28">
-        <v>342.26</v>
+        <v>362.1</v>
       </c>
       <c r="S28">
-        <v>138.88</v>
+        <v>158.72</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
@@ -4217,7 +4217,7 @@
         <v>131.5</v>
       </c>
       <c r="E29">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F29">
         <v>10.11</v>
@@ -4253,13 +4253,13 @@
         <v>363.5</v>
       </c>
       <c r="Q29">
-        <v>-342.33000000000004</v>
+        <v>-372.65999999999997</v>
       </c>
       <c r="R29">
         <v>-210.9</v>
       </c>
       <c r="S29">
-        <v>131.43</v>
+        <v>161.76</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
@@ -4453,7 +4453,7 @@
         <v>131.5</v>
       </c>
       <c r="E33">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F33">
         <v>10.11</v>
@@ -4492,10 +4492,10 @@
         <v>210.9</v>
       </c>
       <c r="R33">
-        <v>342.33000000000004</v>
+        <v>372.65999999999997</v>
       </c>
       <c r="S33">
-        <v>131.43</v>
+        <v>161.76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>